<commit_message>
Final Thesis Push (Clean Reset)
</commit_message>
<xml_diff>
--- a/Medical_AI_90_Day_Plan.xlsx
+++ b/Medical_AI_90_Day_Plan.xlsx
@@ -1855,7 +1855,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1873,6 +1873,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2229,8 +2232,8 @@
   <sheetPr/>
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -2421,7 +2424,7 @@
       <c r="E8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -2490,7 +2493,7 @@
       <c r="E11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>57</v>
       </c>
       <c r="G11" s="6" t="s">
@@ -2513,7 +2516,7 @@
       <c r="E12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>61</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -2521,22 +2524,22 @@
       </c>
     </row>
     <row r="13" ht="25" customHeight="1" spans="1:7">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>65</v>
       </c>
       <c r="G13" s="6" t="s">
@@ -2544,22 +2547,22 @@
       </c>
     </row>
     <row r="14" ht="25" customHeight="1" spans="1:7">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>69</v>
       </c>
       <c r="G14" s="6" t="s">
@@ -2567,22 +2570,22 @@
       </c>
     </row>
     <row r="15" ht="25" customHeight="1" spans="1:7">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G15" s="6" t="s">
@@ -2590,22 +2593,22 @@
       </c>
     </row>
     <row r="16" ht="25" customHeight="1" spans="1:7">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G16" s="6" t="s">
@@ -2613,13 +2616,13 @@
       </c>
     </row>
     <row r="17" ht="25" customHeight="1" spans="1:7">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -2628,7 +2631,7 @@
       <c r="E17" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>84</v>
       </c>
       <c r="G17" s="6" t="s">
@@ -2636,13 +2639,13 @@
       </c>
     </row>
     <row r="18" ht="25" customHeight="1" spans="1:7">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -2651,7 +2654,7 @@
       <c r="E18" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>88</v>
       </c>
       <c r="G18" s="6" t="s">
@@ -2659,13 +2662,13 @@
       </c>
     </row>
     <row r="19" ht="25" customHeight="1" spans="1:7">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="8" t="s">
         <v>90</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -2674,7 +2677,7 @@
       <c r="E19" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>93</v>
       </c>
       <c r="G19" s="6" t="s">
@@ -2682,13 +2685,13 @@
       </c>
     </row>
     <row r="20" ht="25" customHeight="1" spans="1:7">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="8" t="s">
         <v>94</v>
       </c>
       <c r="D20" s="6" t="s">
@@ -2697,7 +2700,7 @@
       <c r="E20" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>97</v>
       </c>
       <c r="G20" s="6" t="s">
@@ -2705,19 +2708,19 @@
       </c>
     </row>
     <row r="21" ht="25" customHeight="1" spans="1:7">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="8" t="s">
         <v>98</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="9" t="s">
         <v>100</v>
       </c>
       <c r="F21" s="6" t="s">
@@ -2728,13 +2731,13 @@
       </c>
     </row>
     <row r="22" ht="25" customHeight="1" spans="1:7">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="8" t="s">
         <v>102</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -2743,7 +2746,7 @@
       <c r="E22" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>105</v>
       </c>
       <c r="G22" s="6" t="s">
@@ -2751,13 +2754,13 @@
       </c>
     </row>
     <row r="23" ht="25" customHeight="1" spans="1:7">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="8" t="s">
         <v>107</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -2766,7 +2769,7 @@
       <c r="E23" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="5" t="s">
         <v>110</v>
       </c>
       <c r="G23" s="6" t="s">
@@ -2774,13 +2777,13 @@
       </c>
     </row>
     <row r="24" ht="25" customHeight="1" spans="1:7">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="8" t="s">
         <v>112</v>
       </c>
       <c r="D24" s="6" t="s">
@@ -2789,7 +2792,7 @@
       <c r="E24" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>115</v>
       </c>
       <c r="G24" s="6" t="s">
@@ -2797,13 +2800,13 @@
       </c>
     </row>
     <row r="25" ht="25" customHeight="1" spans="1:7">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="8" t="s">
         <v>116</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -2812,7 +2815,7 @@
       <c r="E25" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>119</v>
       </c>
       <c r="G25" s="6" t="s">
@@ -2820,13 +2823,13 @@
       </c>
     </row>
     <row r="26" ht="25" customHeight="1" spans="1:7">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="8" t="s">
         <v>120</v>
       </c>
       <c r="D26" s="6" t="s">
@@ -2835,7 +2838,7 @@
       <c r="E26" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>123</v>
       </c>
       <c r="G26" s="6" t="s">
@@ -2843,13 +2846,13 @@
       </c>
     </row>
     <row r="27" ht="25" customHeight="1" spans="1:7">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="8" t="s">
         <v>124</v>
       </c>
       <c r="D27" s="6" t="s">
@@ -2866,13 +2869,13 @@
       </c>
     </row>
     <row r="28" ht="25" customHeight="1" spans="1:7">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="8" t="s">
         <v>128</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -2889,13 +2892,13 @@
       </c>
     </row>
     <row r="29" ht="25" customHeight="1" spans="1:7">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="8" t="s">
         <v>132</v>
       </c>
       <c r="D29" s="6" t="s">
@@ -2912,13 +2915,13 @@
       </c>
     </row>
     <row r="30" ht="25" customHeight="1" spans="1:7">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="8" t="s">
         <v>136</v>
       </c>
       <c r="D30" s="6" t="s">
@@ -2935,13 +2938,13 @@
       </c>
     </row>
     <row r="31" ht="25" customHeight="1" spans="1:7">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="8" t="s">
         <v>138</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -2958,13 +2961,13 @@
       </c>
     </row>
     <row r="32" ht="25" customHeight="1" spans="1:7">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="8" t="s">
         <v>144</v>
       </c>
       <c r="D32" s="6" t="s">
@@ -2981,19 +2984,19 @@
       </c>
     </row>
     <row r="33" ht="25" customHeight="1" spans="1:7">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="8" t="s">
         <v>149</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="9" t="s">
         <v>151</v>
       </c>
       <c r="F33" s="6" t="s">
@@ -3004,13 +3007,13 @@
       </c>
     </row>
     <row r="34" ht="25" customHeight="1" spans="1:7">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="8" t="s">
         <v>154</v>
       </c>
       <c r="D34" s="6" t="s">
@@ -3027,19 +3030,19 @@
       </c>
     </row>
     <row r="35" ht="25" customHeight="1" spans="1:7">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="8" t="s">
         <v>159</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="9" t="s">
         <v>161</v>
       </c>
       <c r="F35" s="6" t="s">
@@ -3050,13 +3053,13 @@
       </c>
     </row>
     <row r="36" ht="25" customHeight="1" spans="1:7">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="8" t="s">
         <v>163</v>
       </c>
       <c r="D36" s="6" t="s">
@@ -3073,13 +3076,13 @@
       </c>
     </row>
     <row r="37" ht="25" customHeight="1" spans="1:7">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="8" t="s">
         <v>168</v>
       </c>
       <c r="D37" s="6" t="s">
@@ -3096,13 +3099,13 @@
       </c>
     </row>
     <row r="38" ht="25" customHeight="1" spans="1:7">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="8" t="s">
         <v>172</v>
       </c>
       <c r="D38" s="6" t="s">
@@ -3119,19 +3122,19 @@
       </c>
     </row>
     <row r="39" ht="25" customHeight="1" spans="1:7">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="8" t="s">
         <v>178</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="9" t="s">
         <v>180</v>
       </c>
       <c r="F39" s="6" t="s">
@@ -3142,13 +3145,13 @@
       </c>
     </row>
     <row r="40" ht="25" customHeight="1" spans="1:7">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="8" t="s">
         <v>183</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -3165,13 +3168,13 @@
       </c>
     </row>
     <row r="41" ht="25" customHeight="1" spans="1:7">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="8" t="s">
         <v>187</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -3188,13 +3191,13 @@
       </c>
     </row>
     <row r="42" ht="25" customHeight="1" spans="1:7">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="8" t="s">
         <v>191</v>
       </c>
       <c r="D42" s="6" t="s">
@@ -3211,13 +3214,13 @@
       </c>
     </row>
     <row r="43" ht="25" customHeight="1" spans="1:7">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="8" t="s">
         <v>196</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -3234,13 +3237,13 @@
       </c>
     </row>
     <row r="44" ht="25" customHeight="1" spans="1:7">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="8" t="s">
         <v>200</v>
       </c>
       <c r="D44" s="6" t="s">
@@ -3257,13 +3260,13 @@
       </c>
     </row>
     <row r="45" ht="25" customHeight="1" spans="1:7">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="8" t="s">
         <v>204</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -3280,13 +3283,13 @@
       </c>
     </row>
     <row r="46" ht="25" customHeight="1" spans="1:7">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="8" t="s">
         <v>209</v>
       </c>
       <c r="D46" s="6" t="s">
@@ -3303,13 +3306,13 @@
       </c>
     </row>
     <row r="47" ht="25" customHeight="1" spans="1:7">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="8" t="s">
         <v>213</v>
       </c>
       <c r="D47" s="6" t="s">
@@ -3326,13 +3329,13 @@
       </c>
     </row>
     <row r="48" ht="25" customHeight="1" spans="1:7">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="8" t="s">
         <v>217</v>
       </c>
       <c r="D48" s="6" t="s">
@@ -3349,13 +3352,13 @@
       </c>
     </row>
     <row r="49" ht="25" customHeight="1" spans="1:7">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="8" t="s">
         <v>221</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -3372,13 +3375,13 @@
       </c>
     </row>
     <row r="50" ht="25" customHeight="1" spans="1:7">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="8" t="s">
         <v>225</v>
       </c>
       <c r="D50" s="6" t="s">
@@ -3395,13 +3398,13 @@
       </c>
     </row>
     <row r="51" ht="25" customHeight="1" spans="1:7">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="8" t="s">
         <v>229</v>
       </c>
       <c r="D51" s="6" t="s">
@@ -3418,13 +3421,13 @@
       </c>
     </row>
     <row r="52" ht="25" customHeight="1" spans="1:7">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="8" t="s">
         <v>233</v>
       </c>
       <c r="D52" s="6" t="s">
@@ -3441,13 +3444,13 @@
       </c>
     </row>
     <row r="53" ht="25" customHeight="1" spans="1:7">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="8" t="s">
         <v>239</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -3464,13 +3467,13 @@
       </c>
     </row>
     <row r="54" ht="25" customHeight="1" spans="1:7">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="8" t="s">
         <v>243</v>
       </c>
       <c r="D54" s="6" t="s">
@@ -3487,13 +3490,13 @@
       </c>
     </row>
     <row r="55" ht="25" customHeight="1" spans="1:7">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="8" t="s">
         <v>247</v>
       </c>
       <c r="D55" s="6" t="s">
@@ -3510,13 +3513,13 @@
       </c>
     </row>
     <row r="56" ht="25" customHeight="1" spans="1:7">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="8" t="s">
         <v>251</v>
       </c>
       <c r="D56" s="6" t="s">
@@ -3533,13 +3536,13 @@
       </c>
     </row>
     <row r="57" ht="25" customHeight="1" spans="1:7">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="8" t="s">
         <v>255</v>
       </c>
       <c r="D57" s="6" t="s">
@@ -3556,13 +3559,13 @@
       </c>
     </row>
     <row r="58" ht="25" customHeight="1" spans="1:7">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="8" t="s">
         <v>259</v>
       </c>
       <c r="D58" s="6" t="s">
@@ -3579,13 +3582,13 @@
       </c>
     </row>
     <row r="59" ht="25" customHeight="1" spans="1:7">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="8" t="s">
         <v>263</v>
       </c>
       <c r="D59" s="6" t="s">
@@ -3602,13 +3605,13 @@
       </c>
     </row>
     <row r="60" ht="25" customHeight="1" spans="1:7">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="8" t="s">
         <v>267</v>
       </c>
       <c r="D60" s="6" t="s">
@@ -3625,13 +3628,13 @@
       </c>
     </row>
     <row r="61" ht="25" customHeight="1" spans="1:7">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="8" t="s">
         <v>271</v>
       </c>
       <c r="D61" s="6" t="s">
@@ -3648,13 +3651,13 @@
       </c>
     </row>
     <row r="62" ht="25" customHeight="1" spans="1:7">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="8" t="s">
         <v>277</v>
       </c>
       <c r="D62" s="6" t="s">
@@ -3671,13 +3674,13 @@
       </c>
     </row>
     <row r="63" ht="25" customHeight="1" spans="1:7">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="8" t="s">
         <v>282</v>
       </c>
       <c r="D63" s="6" t="s">
@@ -3694,13 +3697,13 @@
       </c>
     </row>
     <row r="64" ht="25" customHeight="1" spans="1:7">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="8" t="s">
         <v>286</v>
       </c>
       <c r="D64" s="6" t="s">
@@ -3717,13 +3720,13 @@
       </c>
     </row>
     <row r="65" ht="25" customHeight="1" spans="1:7">
-      <c r="A65" s="7" t="s">
+      <c r="A65" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="8" t="s">
         <v>290</v>
       </c>
       <c r="D65" s="6" t="s">
@@ -3740,13 +3743,13 @@
       </c>
     </row>
     <row r="66" ht="25" customHeight="1" spans="1:7">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="8" t="s">
         <v>294</v>
       </c>
       <c r="D66" s="6" t="s">
@@ -3763,13 +3766,13 @@
       </c>
     </row>
     <row r="67" ht="25" customHeight="1" spans="1:7">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C67" s="8" t="s">
         <v>297</v>
       </c>
       <c r="D67" s="6" t="s">
@@ -3786,13 +3789,13 @@
       </c>
     </row>
     <row r="68" ht="25" customHeight="1" spans="1:7">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C68" s="8" t="s">
         <v>300</v>
       </c>
       <c r="D68" s="6" t="s">
@@ -3809,13 +3812,13 @@
       </c>
     </row>
     <row r="69" ht="25" customHeight="1" spans="1:7">
-      <c r="A69" s="7" t="s">
+      <c r="A69" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="8" t="s">
         <v>305</v>
       </c>
       <c r="D69" s="6" t="s">
@@ -3832,13 +3835,13 @@
       </c>
     </row>
     <row r="70" ht="25" customHeight="1" spans="1:7">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C70" s="8" t="s">
         <v>309</v>
       </c>
       <c r="D70" s="6" t="s">
@@ -3855,13 +3858,13 @@
       </c>
     </row>
     <row r="71" ht="25" customHeight="1" spans="1:7">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C71" s="8" t="s">
         <v>313</v>
       </c>
       <c r="D71" s="6" t="s">
@@ -3878,13 +3881,13 @@
       </c>
     </row>
     <row r="72" ht="25" customHeight="1" spans="1:7">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="8" t="s">
         <v>317</v>
       </c>
       <c r="D72" s="6" t="s">
@@ -3901,13 +3904,13 @@
       </c>
     </row>
     <row r="73" ht="25" customHeight="1" spans="1:7">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B73" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="C73" s="8" t="s">
         <v>321</v>
       </c>
       <c r="D73" s="6" t="s">
@@ -3924,13 +3927,13 @@
       </c>
     </row>
     <row r="74" ht="25" customHeight="1" spans="1:7">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B74" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="C74" s="8" t="s">
         <v>325</v>
       </c>
       <c r="D74" s="6" t="s">
@@ -3947,13 +3950,13 @@
       </c>
     </row>
     <row r="75" ht="25" customHeight="1" spans="1:7">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B75" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="C75" s="8" t="s">
         <v>329</v>
       </c>
       <c r="D75" s="6" t="s">
@@ -3970,13 +3973,13 @@
       </c>
     </row>
     <row r="76" ht="25" customHeight="1" spans="1:7">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="8" t="s">
         <v>333</v>
       </c>
       <c r="D76" s="6" t="s">
@@ -3993,13 +3996,13 @@
       </c>
     </row>
     <row r="77" ht="25" customHeight="1" spans="1:7">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B77" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C77" s="8" t="s">
         <v>337</v>
       </c>
       <c r="D77" s="6" t="s">
@@ -4016,13 +4019,13 @@
       </c>
     </row>
     <row r="78" ht="25" customHeight="1" spans="1:7">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B78" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C78" s="8" t="s">
         <v>340</v>
       </c>
       <c r="D78" s="6" t="s">
@@ -4039,13 +4042,13 @@
       </c>
     </row>
     <row r="79" ht="25" customHeight="1" spans="1:7">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B79" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C79" s="8" t="s">
         <v>343</v>
       </c>
       <c r="D79" s="6" t="s">
@@ -4062,13 +4065,13 @@
       </c>
     </row>
     <row r="80" ht="25" customHeight="1" spans="1:7">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C80" s="8" t="s">
         <v>347</v>
       </c>
       <c r="D80" s="6" t="s">
@@ -4085,13 +4088,13 @@
       </c>
     </row>
     <row r="81" ht="25" customHeight="1" spans="1:7">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B81" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="C81" s="7" t="s">
+      <c r="C81" s="8" t="s">
         <v>351</v>
       </c>
       <c r="D81" s="6" t="s">
@@ -4108,13 +4111,13 @@
       </c>
     </row>
     <row r="82" ht="25" customHeight="1" spans="1:7">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B82" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="C82" s="8" t="s">
         <v>355</v>
       </c>
       <c r="D82" s="6" t="s">
@@ -4131,13 +4134,13 @@
       </c>
     </row>
     <row r="83" ht="25" customHeight="1" spans="1:7">
-      <c r="A83" s="7" t="s">
+      <c r="A83" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B83" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C83" s="7" t="s">
+      <c r="C83" s="8" t="s">
         <v>358</v>
       </c>
       <c r="D83" s="6" t="s">
@@ -4154,13 +4157,13 @@
       </c>
     </row>
     <row r="84" ht="25" customHeight="1" spans="1:7">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="B84" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C84" s="7" t="s">
+      <c r="C84" s="8" t="s">
         <v>362</v>
       </c>
       <c r="D84" s="6" t="s">
@@ -4177,13 +4180,13 @@
       </c>
     </row>
     <row r="85" ht="25" customHeight="1" spans="1:7">
-      <c r="A85" s="7" t="s">
+      <c r="A85" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B85" s="7" t="s">
+      <c r="B85" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C85" s="8" t="s">
         <v>366</v>
       </c>
       <c r="D85" s="6" t="s">
@@ -4200,13 +4203,13 @@
       </c>
     </row>
     <row r="86" ht="25" customHeight="1" spans="1:7">
-      <c r="A86" s="7" t="s">
+      <c r="A86" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B86" s="7" t="s">
+      <c r="B86" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C86" s="8" t="s">
         <v>370</v>
       </c>
       <c r="D86" s="6" t="s">
@@ -4223,13 +4226,13 @@
       </c>
     </row>
     <row r="87" ht="25" customHeight="1" spans="1:7">
-      <c r="A87" s="7" t="s">
+      <c r="A87" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="B87" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="C87" s="8" t="s">
         <v>374</v>
       </c>
       <c r="D87" s="6" t="s">
@@ -4246,13 +4249,13 @@
       </c>
     </row>
     <row r="88" ht="25" customHeight="1" spans="1:7">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B88" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C88" s="8" t="s">
         <v>378</v>
       </c>
       <c r="D88" s="6" t="s">
@@ -4269,13 +4272,13 @@
       </c>
     </row>
     <row r="89" ht="25" customHeight="1" spans="1:7">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B89" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="C89" s="8" t="s">
         <v>382</v>
       </c>
       <c r="D89" s="6" t="s">
@@ -4292,13 +4295,13 @@
       </c>
     </row>
     <row r="90" ht="25" customHeight="1" spans="1:7">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="B90" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C90" s="7" t="s">
+      <c r="C90" s="8" t="s">
         <v>385</v>
       </c>
       <c r="D90" s="6" t="s">
@@ -4315,13 +4318,13 @@
       </c>
     </row>
     <row r="91" ht="25" customHeight="1" spans="1:7">
-      <c r="A91" s="7" t="s">
+      <c r="A91" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="B91" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="C91" s="8" t="s">
         <v>388</v>
       </c>
       <c r="D91" s="6" t="s">

</xml_diff>